<commit_message>
Added work break down structure (WIP) Updated scrum board Added review log for bernardo's work
</commit_message>
<xml_diff>
--- a/Scrum Board.xlsx
+++ b/Scrum Board.xlsx
@@ -28,31 +28,31 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>Setup the GanttProject. This includes forking the repository from GitHub</t>
+    <t>(ID: 'A') Setup the GanttProject. This includes forking the repository from GitHub</t>
   </si>
   <si>
     <t>Create Fork</t>
   </si>
   <si>
-    <t>Identify pinpoint code smells used to design this tool</t>
+    <t>(ID: 'B') Identify pinpoint code smells used to design this tool</t>
   </si>
   <si>
     <t>Clone the project.</t>
   </si>
   <si>
-    <t>Identify GoF Design patterns used to design this tool</t>
+    <t>(ID: 'C') Identify GoF Design patterns used to design this tool</t>
   </si>
   <si>
     <t>Everyone checks three code smells.</t>
   </si>
   <si>
-    <t>Each team member should review three other colleague´s code smells.</t>
+    <t>(ID: 'D') Each team member should review three other colleague´s code smells.</t>
   </si>
   <si>
     <t>Everyone checks three design patterns.</t>
   </si>
   <si>
-    <t>Each team member should review three other colleague´s design patterns.</t>
+    <t>(ID: 'E') Each team member should review three other colleague´s design patterns.</t>
   </si>
   <si>
     <t>Everyone reviews three code smells from another colleague.</t>
@@ -426,10 +426,10 @@
         <v>13</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="7"/>
+      <c r="H16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="8"/>
       <c r="J16" s="8"/>
     </row>
     <row r="19">
@@ -515,41 +515,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="F4:G6"/>
+    <mergeCell ref="H4:I6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I6"/>
-    <mergeCell ref="H7:I9"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D4:E6"/>
+    <mergeCell ref="J4:K6"/>
+    <mergeCell ref="H10:I12"/>
+    <mergeCell ref="J10:K12"/>
+    <mergeCell ref="H13:I15"/>
+    <mergeCell ref="J13:K15"/>
     <mergeCell ref="H16:I18"/>
-    <mergeCell ref="H19:I21"/>
-    <mergeCell ref="H10:I12"/>
-    <mergeCell ref="H13:I15"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K6"/>
-    <mergeCell ref="J7:K9"/>
     <mergeCell ref="J16:K18"/>
-    <mergeCell ref="J19:K21"/>
-    <mergeCell ref="J10:K12"/>
-    <mergeCell ref="J13:K15"/>
-    <mergeCell ref="F10:G12"/>
-    <mergeCell ref="F13:G15"/>
-    <mergeCell ref="F19:G21"/>
-    <mergeCell ref="B10:C12"/>
-    <mergeCell ref="B13:C15"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C6"/>
     <mergeCell ref="B7:C9"/>
-    <mergeCell ref="D10:E12"/>
-    <mergeCell ref="D13:E15"/>
-    <mergeCell ref="D16:E18"/>
-    <mergeCell ref="D19:E21"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E6"/>
     <mergeCell ref="D7:E9"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G6"/>
     <mergeCell ref="F7:G9"/>
-    <mergeCell ref="F16:G18"/>
+    <mergeCell ref="H7:I9"/>
+    <mergeCell ref="J7:K9"/>
+    <mergeCell ref="B10:C12"/>
     <mergeCell ref="B16:C18"/>
     <mergeCell ref="B19:C21"/>
+    <mergeCell ref="D19:E21"/>
+    <mergeCell ref="F19:G21"/>
+    <mergeCell ref="H19:I21"/>
+    <mergeCell ref="J19:K21"/>
+    <mergeCell ref="F16:G18"/>
+    <mergeCell ref="D10:E12"/>
+    <mergeCell ref="F10:G12"/>
+    <mergeCell ref="B13:C15"/>
+    <mergeCell ref="D13:E15"/>
+    <mergeCell ref="F13:G15"/>
+    <mergeCell ref="D16:E18"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>